<commit_message>
writing report test docs...and discovering issues along the way
git-svn-id: svn://localhost/ARK/trunk@8200 35ee9b83-dd2c-47f4-99a2-c706670c48ce
</commit_message>
<xml_diff>
--- a/usefulTools/TestFilesAndDocuments/UAT_Reporting_Data_Linkage_Requirements_no_results.xlsx
+++ b/usefulTools/TestFilesAndDocuments/UAT_Reporting_Data_Linkage_Requirements_no_results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Result coding: 1 = Pass (full functionality with no unexpected errors), 0 = Fail (lack of required functionality or reproducible error during testing), 9 = Conditional (partial functionality, error during testing which cannot be reproduced, poor user experience or other constraints) X = Functionality which is desirable for future iterations of the system. these items are not necessary for user acceptance of this version of the system</t>
   </si>
@@ -51,7 +51,7 @@
     <t>STUDIES</t>
   </si>
   <si>
-    <t>2.1</t>
+    <t>1.1</t>
   </si>
   <si>
     <r>
@@ -72,70 +72,73 @@
     </r>
   </si>
   <si>
-    <t>2.2</t>
+    <t>1.2</t>
   </si>
   <si>
     <t>a user with appropriate access rights can access the reporting module</t>
   </si>
   <si>
-    <t>2.3</t>
+    <t>1.3</t>
   </si>
   <si>
     <t>a user with appropriate access rights can access the report tab within the reporting module</t>
   </si>
   <si>
-    <t>2.4</t>
+    <t>1.4</t>
   </si>
   <si>
     <t>a user with appropriate access rights can access the Study Summary Report</t>
   </si>
   <si>
-    <t>2.5</t>
+    <t>1.5</t>
   </si>
   <si>
     <t>a user withOUT appropriate access rights can NOT access the Study Summary Report</t>
   </si>
   <si>
-    <t>2.6</t>
+    <t>1.6</t>
   </si>
   <si>
     <t>a user withOUT appropriate access rights can NOT access the report tab</t>
   </si>
   <si>
-    <t>2.7</t>
+    <t>1.7</t>
   </si>
   <si>
     <t>Produce a study summary report – confirm that pdf and csv report are produced...and for each;</t>
   </si>
   <si>
-    <t>2.8</t>
+    <t>1.8</t>
   </si>
   <si>
     <t>confirm that the subject data matches what is seen in the study details tab of the study module</t>
   </si>
   <si>
-    <t>2.9</t>
+    <t>1.9</t>
   </si>
   <si>
     <t>Add a subject.  Immediately - Re-run the report.  Confirm that the subject count has incremented by one.</t>
   </si>
   <si>
-    <t>2.10</t>
+    <t>1.10</t>
   </si>
   <si>
     <t>remove added subject ( or another test subject ) and check that the amount of subject is adequate decremented by one</t>
   </si>
   <si>
-    <t>2.11</t>
+    <t>1.11</t>
   </si>
   <si>
     <t>change study-consent state in multiple ways and check that the consented and non-consented  counts are adjusted appropriately</t>
   </si>
   <si>
-    <t>2.12</t>
+    <t>1.12</t>
   </si>
   <si>
     <t>alter consent to specific components and see that it appopriately increments and decrements the component-specific-constent counts</t>
+  </si>
+  <si>
+    <t>Study-level Consent Details Report</t>
   </si>
   <si>
     <t>to be disussed</t>
@@ -342,7 +345,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
@@ -445,6 +448,10 @@
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="0" fontId="10" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="0" fontId="11" numFmtId="164" xfId="0">
@@ -620,8 +627,8 @@
   </sheetPr>
   <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100">
-      <selection activeCell="B18" activeCellId="0" pane="topLeft" sqref="B18"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100">
+      <selection activeCell="B19" activeCellId="0" pane="topLeft" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -699,9 +706,6 @@
       <c r="M4" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="5">
-      <c r="A5" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="B5" s="21" t="s">
         <v>10</v>
       </c>
@@ -903,7 +907,9 @@
       <c r="I18" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="150.75" outlineLevel="0" r="19">
-      <c r="B19" s="30"/>
+      <c r="B19" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="C19" s="27"/>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
@@ -957,7 +963,7 @@
       <c r="E24" s="27"/>
       <c r="F24" s="24"/>
       <c r="G24" s="25"/>
-      <c r="H24" s="32"/>
+      <c r="H24" s="33"/>
       <c r="I24" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="73.5" outlineLevel="0" r="25">
@@ -997,7 +1003,7 @@
       <c r="E28" s="30"/>
       <c r="F28" s="24"/>
       <c r="G28" s="25"/>
-      <c r="H28" s="32"/>
+      <c r="H28" s="33"/>
       <c r="I28" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="171.35" outlineLevel="0" r="29">
@@ -1007,10 +1013,10 @@
       <c r="E29" s="30"/>
       <c r="F29" s="24"/>
       <c r="G29" s="25"/>
-      <c r="H29" s="32"/>
+      <c r="H29" s="33"/>
       <c r="I29" s="26"/>
       <c r="J29" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="153" outlineLevel="0" r="30">
@@ -1034,7 +1040,7 @@
       <c r="I31" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="124.5" outlineLevel="0" r="32">
-      <c r="B32" s="33"/>
+      <c r="B32" s="34"/>
       <c r="C32" s="27"/>
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
@@ -1044,27 +1050,27 @@
       <c r="I32" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="109.5" outlineLevel="0" r="33">
-      <c r="B33" s="33"/>
+      <c r="B33" s="34"/>
       <c r="C33" s="27"/>
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
       <c r="F33" s="24"/>
       <c r="G33" s="25"/>
-      <c r="H33" s="32"/>
+      <c r="H33" s="33"/>
       <c r="I33" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="93.75" outlineLevel="0" r="34">
-      <c r="B34" s="33"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="27"/>
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
       <c r="F34" s="24"/>
       <c r="G34" s="25"/>
-      <c r="H34" s="32"/>
+      <c r="H34" s="33"/>
       <c r="I34" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="109.5" outlineLevel="0" r="35">
-      <c r="B35" s="33"/>
+      <c r="B35" s="34"/>
       <c r="C35" s="27"/>
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
@@ -1074,7 +1080,7 @@
       <c r="I35" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="124.5" outlineLevel="0" r="36">
-      <c r="B36" s="33"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="27"/>
       <c r="D36" s="27"/>
       <c r="E36" s="27"/>
@@ -1084,7 +1090,7 @@
       <c r="I36" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="124.5" outlineLevel="0" r="37">
-      <c r="B37" s="33"/>
+      <c r="B37" s="34"/>
       <c r="C37" s="27"/>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
@@ -1094,14 +1100,14 @@
       <c r="I37" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
-      <c r="B38" s="34"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
+      <c r="B38" s="35"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="99.95" outlineLevel="0" r="39">
-      <c r="B39" s="36"/>
+      <c r="B39" s="37"/>
       <c r="C39" s="27"/>
       <c r="D39" s="27"/>
       <c r="E39" s="27"/>
@@ -1111,7 +1117,7 @@
       <c r="I39" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="99.95" outlineLevel="0" r="40">
-      <c r="B40" s="36"/>
+      <c r="B40" s="37"/>
       <c r="C40" s="27"/>
       <c r="D40" s="27"/>
       <c r="E40" s="27"/>
@@ -1121,7 +1127,7 @@
       <c r="I40" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="99.95" outlineLevel="0" r="41">
-      <c r="B41" s="36"/>
+      <c r="B41" s="37"/>
       <c r="C41" s="27"/>
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
@@ -1131,7 +1137,7 @@
       <c r="I41" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="99.95" outlineLevel="0" r="42">
-      <c r="B42" s="36"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="27"/>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
@@ -1141,7 +1147,7 @@
       <c r="I42" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="99.95" outlineLevel="0" r="43">
-      <c r="B43" s="36"/>
+      <c r="B43" s="37"/>
       <c r="C43" s="27"/>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
@@ -1151,7 +1157,7 @@
       <c r="I43" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="99.95" outlineLevel="0" r="44">
-      <c r="B44" s="36"/>
+      <c r="B44" s="37"/>
       <c r="C44" s="27"/>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
@@ -1161,7 +1167,7 @@
       <c r="I44" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="99.95" outlineLevel="0" r="45">
-      <c r="B45" s="36"/>
+      <c r="B45" s="37"/>
       <c r="C45" s="27"/>
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
@@ -1176,9 +1182,9 @@
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
       <c r="E46" s="18"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="39"/>
       <c r="I46" s="20"/>
       <c r="J46" s="16"/>
       <c r="K46" s="16"/>
@@ -1186,33 +1192,33 @@
       <c r="M46" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="47">
-      <c r="B47" s="34"/>
+      <c r="B47" s="35"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="48">
-      <c r="B48" s="34"/>
+      <c r="B48" s="35"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="75.75" outlineLevel="0" r="49">
-      <c r="B49" s="36"/>
+      <c r="B49" s="37"/>
       <c r="C49" s="27"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="40"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
       <c r="F49" s="24"/>
       <c r="G49" s="24"/>
       <c r="H49" s="23"/>
       <c r="I49" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="70.5" outlineLevel="0" r="50">
-      <c r="B50" s="36"/>
+      <c r="B50" s="37"/>
       <c r="C50" s="27"/>
       <c r="D50" s="27"/>
       <c r="E50" s="27"/>
@@ -1222,23 +1228,23 @@
       <c r="I50" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="51">
-      <c r="B51" s="36"/>
-      <c r="C51" s="40"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="41"/>
       <c r="F51" s="24"/>
       <c r="G51" s="24"/>
-      <c r="H51" s="41"/>
+      <c r="H51" s="42"/>
       <c r="I51" s="26"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="45.75" outlineLevel="0" r="52" s="48">
-      <c r="A52" s="42"/>
-      <c r="B52" s="43"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="45"/>
-      <c r="G52" s="45"/>
-      <c r="H52" s="46"/>
-      <c r="I52" s="47"/>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="45.75" outlineLevel="0" r="52" s="49">
+      <c r="A52" s="43"/>
+      <c r="B52" s="44"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="46"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="47"/>
+      <c r="I52" s="48"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="53">
       <c r="A53" s="15"/>
@@ -1246,9 +1252,9 @@
       <c r="C53" s="17"/>
       <c r="D53" s="17"/>
       <c r="E53" s="18"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="39"/>
       <c r="I53" s="20"/>
       <c r="J53" s="16"/>
       <c r="K53" s="16"/>
@@ -1256,22 +1262,22 @@
       <c r="M53" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="54">
-      <c r="B54" s="34"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
+      <c r="B54" s="35"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="55">
-      <c r="B55" s="34"/>
+      <c r="B55" s="35"/>
       <c r="F55" s="22"/>
       <c r="G55" s="22"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="61.5" outlineLevel="0" r="56">
-      <c r="B56" s="36"/>
+      <c r="B56" s="37"/>
       <c r="C56" s="30"/>
       <c r="D56" s="27"/>
       <c r="E56" s="27"/>
       <c r="F56" s="24"/>
-      <c r="G56" s="49"/>
+      <c r="G56" s="50"/>
       <c r="H56" s="23"/>
       <c r="I56" s="26"/>
     </row>
@@ -1281,9 +1287,9 @@
       <c r="C57" s="17"/>
       <c r="D57" s="17"/>
       <c r="E57" s="18"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="38"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="39"/>
       <c r="I57" s="20"/>
       <c r="J57" s="16"/>
       <c r="K57" s="16"/>
@@ -1291,47 +1297,47 @@
       <c r="M57" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="58">
-      <c r="B58" s="34"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
+      <c r="B58" s="35"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="59">
-      <c r="B59" s="34"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
+      <c r="B59" s="35"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="40"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="60">
-      <c r="B60" s="34"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
+      <c r="B60" s="35"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="40"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="73.5" outlineLevel="0" r="61">
-      <c r="B61" s="36"/>
+      <c r="B61" s="37"/>
       <c r="C61" s="27"/>
       <c r="D61" s="27"/>
       <c r="E61" s="27"/>
       <c r="F61" s="24"/>
-      <c r="G61" s="49"/>
+      <c r="G61" s="50"/>
       <c r="H61" s="23"/>
       <c r="I61" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="72" outlineLevel="0" r="62">
-      <c r="B62" s="36"/>
+      <c r="B62" s="37"/>
       <c r="C62" s="27"/>
       <c r="D62" s="27"/>
       <c r="E62" s="27"/>
       <c r="F62" s="24"/>
-      <c r="G62" s="49"/>
+      <c r="G62" s="50"/>
       <c r="H62" s="23"/>
       <c r="I62" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="63">
-      <c r="B63" s="34"/>
-      <c r="F63" s="39"/>
-      <c r="G63" s="39"/>
+      <c r="B63" s="35"/>
+      <c r="F63" s="40"/>
+      <c r="G63" s="40"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="105" outlineLevel="0" r="64">
-      <c r="B64" s="36"/>
+      <c r="B64" s="37"/>
       <c r="C64" s="27"/>
       <c r="D64" s="27"/>
       <c r="E64" s="27"/>
@@ -1341,45 +1347,45 @@
       <c r="I64" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="69.75" outlineLevel="0" r="65">
-      <c r="B65" s="36"/>
+      <c r="B65" s="37"/>
       <c r="C65" s="30"/>
       <c r="F65" s="24"/>
       <c r="G65" s="24"/>
       <c r="H65" s="23"/>
       <c r="I65" s="26"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="66" s="48">
-      <c r="A66" s="42"/>
-      <c r="B66" s="50"/>
-      <c r="C66" s="44"/>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="66" s="49">
+      <c r="A66" s="43"/>
+      <c r="B66" s="51"/>
+      <c r="C66" s="45"/>
       <c r="D66" s="27"/>
       <c r="E66" s="27"/>
-      <c r="F66" s="45"/>
-      <c r="G66" s="45"/>
-      <c r="H66" s="46"/>
-      <c r="I66" s="47"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="64.5" outlineLevel="0" r="67" s="48">
-      <c r="A67" s="42"/>
-      <c r="B67" s="50"/>
-      <c r="C67" s="44"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
+      <c r="I66" s="48"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="64.5" outlineLevel="0" r="67" s="49">
+      <c r="A67" s="43"/>
+      <c r="B67" s="51"/>
+      <c r="C67" s="45"/>
       <c r="D67" s="27"/>
       <c r="E67" s="27"/>
-      <c r="F67" s="45"/>
-      <c r="G67" s="45"/>
-      <c r="H67" s="46"/>
-      <c r="I67" s="47"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="68" s="48">
-      <c r="A68" s="42"/>
-      <c r="B68" s="50"/>
-      <c r="C68" s="44"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="46"/>
+      <c r="H67" s="47"/>
+      <c r="I67" s="48"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="68" s="49">
+      <c r="A68" s="43"/>
+      <c r="B68" s="51"/>
+      <c r="C68" s="45"/>
       <c r="D68" s="27"/>
       <c r="E68" s="27"/>
-      <c r="F68" s="45"/>
-      <c r="G68" s="45"/>
-      <c r="H68" s="46"/>
-      <c r="I68" s="47"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="46"/>
+      <c r="H68" s="47"/>
+      <c r="I68" s="48"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="69">
       <c r="A69" s="15"/>
@@ -1387,9 +1393,9 @@
       <c r="C69" s="17"/>
       <c r="D69" s="17"/>
       <c r="E69" s="18"/>
-      <c r="F69" s="37"/>
-      <c r="G69" s="37"/>
-      <c r="H69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="39"/>
       <c r="I69" s="20"/>
       <c r="J69" s="16"/>
       <c r="K69" s="16"/>
@@ -1397,13 +1403,13 @@
       <c r="M69" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30.75" outlineLevel="0" r="70">
-      <c r="B70" s="51"/>
-      <c r="C70" s="52"/>
-      <c r="F70" s="39"/>
-      <c r="G70" s="39"/>
+      <c r="B70" s="52"/>
+      <c r="C70" s="53"/>
+      <c r="F70" s="40"/>
+      <c r="G70" s="40"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45" outlineLevel="0" r="71">
-      <c r="B71" s="53"/>
+      <c r="B71" s="54"/>
       <c r="F71" s="24"/>
       <c r="G71" s="24"/>
       <c r="H71" s="23"/>
@@ -1415,10 +1421,10 @@
       <c r="C72" s="17"/>
       <c r="D72" s="17"/>
       <c r="E72" s="18"/>
-      <c r="F72" s="54"/>
-      <c r="G72" s="54"/>
-      <c r="H72" s="55"/>
-      <c r="I72" s="56"/>
+      <c r="F72" s="55"/>
+      <c r="G72" s="55"/>
+      <c r="H72" s="56"/>
+      <c r="I72" s="57"/>
       <c r="J72" s="16"/>
       <c r="K72" s="16"/>
       <c r="L72" s="16"/>

</xml_diff>

<commit_message>
significant writing of tests
git-svn-id: svn://localhost/ARK/trunk@8233 35ee9b83-dd2c-47f4-99a2-c706670c48ce
</commit_message>
<xml_diff>
--- a/usefulTools/TestFilesAndDocuments/UAT_Reporting_Data_Linkage_Requirements_no_results.xlsx
+++ b/usefulTools/TestFilesAndDocuments/UAT_Reporting_Data_Linkage_Requirements_no_results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>Result coding: 1 = Pass (full functionality with no unexpected errors), 0 = Fail (lack of required functionality or reproducible error during testing), 9 = Conditional (partial functionality, error during testing which cannot be reproduced, poor user experience or other constraints) X = Functionality which is desirable for future iterations of the system. these items are not necessary for user acceptance of this version of the system</t>
   </si>
@@ -195,6 +195,33 @@
   </si>
   <si>
     <t>Biospecimen and Collection Reporting</t>
+  </si>
+  <si>
+    <t>Biospecimen Summary Report Report</t>
+  </si>
+  <si>
+    <t>a user with appropriate access rights can access the Biospecimen Summar Report</t>
+  </si>
+  <si>
+    <t>a user withOUT appropriate access rights can NOT access the Biospecimen Summary Report</t>
+  </si>
+  <si>
+    <t>Produce a  Biospecimen Summary Report – confirm that pdf and csv report are produced...and for each;</t>
+  </si>
+  <si>
+    <t>Add a biospecimen that matches your report criteria.  Immediately - Re-run the report.  Confirm that the new biospecimen is displayed</t>
+  </si>
+  <si>
+    <t>confirm that the biospecimen data matches what is seen subject biospecimen page by narrowing down on a subject uid.  This includes EVERY FIELD that is displayed</t>
+  </si>
+  <si>
+    <t>Delete the newly added biospecimen and check that the report does not include the deleted biospecimen</t>
+  </si>
+  <si>
+    <t>Biospecimen Detail Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  This report lists the biospecimen study details for the selected study - including location information.  It is essentially the same as the biospecimen summary report but includes the detailled location/inventory information related to each biospecimen (it is worth noting it will take a little longer too as a result)</t>
   </si>
 </sst>
 </file>
@@ -369,8 +396,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -552,19 +585,25 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -962,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMF87"/>
+  <dimension ref="A1:AMF89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1682,7 +1721,7 @@
     </row>
     <row r="57" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="B57" s="32" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F57" s="24"/>
       <c r="G57" s="47"/>
@@ -1700,7 +1739,7 @@
     </row>
     <row r="59" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="B59" s="9" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="F59" s="24"/>
       <c r="G59" s="47"/>
@@ -1709,16 +1748,16 @@
     </row>
     <row r="60" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="B60" s="9" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F60" s="24"/>
       <c r="G60" s="47"/>
       <c r="H60" s="23"/>
       <c r="I60" s="26"/>
     </row>
-    <row r="61" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B61" s="9" t="s">
-        <v>22</v>
+    <row r="61" spans="1:13" ht="30" thickTop="1" thickBot="1">
+      <c r="B61" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="F61" s="24"/>
       <c r="G61" s="47"/>
@@ -1727,7 +1766,7 @@
     </row>
     <row r="62" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B62" s="8" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="F62" s="24"/>
       <c r="G62" s="47"/>
@@ -1736,7 +1775,7 @@
     </row>
     <row r="63" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B63" s="8" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="F63" s="24"/>
       <c r="G63" s="47"/>
@@ -1745,104 +1784,114 @@
     </row>
     <row r="64" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B64" s="8" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="F64" s="24"/>
       <c r="G64" s="47"/>
       <c r="H64" s="23"/>
       <c r="I64" s="26"/>
     </row>
-    <row r="65" spans="1:13" ht="58" thickTop="1" thickBot="1">
-      <c r="B65" s="8" t="s">
-        <v>42</v>
-      </c>
+    <row r="65" spans="1:13" ht="16" thickTop="1" thickBot="1">
+      <c r="B65" s="8"/>
       <c r="F65" s="24"/>
       <c r="G65" s="47"/>
       <c r="H65" s="23"/>
       <c r="I65" s="26"/>
     </row>
-    <row r="66" spans="1:13" ht="30" thickTop="1" thickBot="1">
-      <c r="B66" s="8" t="s">
-        <v>43</v>
+    <row r="66" spans="1:13" ht="16" thickTop="1" thickBot="1">
+      <c r="B66" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="F66" s="24"/>
-      <c r="G66" s="47"/>
+      <c r="G66" s="24"/>
       <c r="H66" s="23"/>
       <c r="I66" s="26"/>
     </row>
-    <row r="67" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B67" s="34"/>
+    <row r="67" spans="1:13" ht="58" thickTop="1" thickBot="1">
+      <c r="B67" s="21" t="s">
+        <v>61</v>
+      </c>
       <c r="F67" s="24"/>
-      <c r="G67" s="47"/>
+      <c r="G67" s="24"/>
       <c r="H67" s="23"/>
       <c r="I67" s="26"/>
     </row>
     <row r="68" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B68" s="34"/>
+      <c r="B68" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="F68" s="24"/>
-      <c r="G68" s="47"/>
+      <c r="G68" s="24"/>
       <c r="H68" s="23"/>
       <c r="I68" s="26"/>
     </row>
     <row r="69" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B69" s="34"/>
+      <c r="B69" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="F69" s="24"/>
-      <c r="G69" s="47"/>
+      <c r="G69" s="24"/>
       <c r="H69" s="23"/>
       <c r="I69" s="26"/>
     </row>
-    <row r="70" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B70" s="34"/>
+    <row r="70" spans="1:13" ht="30" thickTop="1" thickBot="1">
+      <c r="B70" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="F70" s="24"/>
-      <c r="G70" s="47"/>
+      <c r="G70" s="24"/>
       <c r="H70" s="23"/>
       <c r="I70" s="26"/>
     </row>
-    <row r="71" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B71" s="36"/>
-      <c r="C71" s="30"/>
-      <c r="D71" s="27"/>
-      <c r="E71" s="27"/>
+    <row r="71" spans="1:13" ht="30" thickTop="1" thickBot="1">
+      <c r="B71" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="F71" s="24"/>
-      <c r="G71" s="47"/>
+      <c r="G71" s="24"/>
       <c r="H71" s="23"/>
       <c r="I71" s="26"/>
     </row>
-    <row r="72" spans="1:13" ht="15" thickTop="1">
-      <c r="A72" s="15"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="37"/>
-      <c r="G72" s="37"/>
-      <c r="H72" s="38"/>
-      <c r="I72" s="20"/>
-      <c r="J72" s="16"/>
-      <c r="K72" s="16"/>
-      <c r="L72" s="16"/>
-      <c r="M72" s="16"/>
-    </row>
-    <row r="73" spans="1:13">
-      <c r="B73" s="34"/>
-      <c r="F73" s="39"/>
-      <c r="G73" s="39"/>
-    </row>
-    <row r="74" spans="1:13">
-      <c r="B74" s="34"/>
-      <c r="F74" s="39"/>
-      <c r="G74" s="39"/>
-    </row>
-    <row r="75" spans="1:13" ht="15" thickBot="1">
-      <c r="B75" s="34"/>
-      <c r="F75" s="39"/>
-      <c r="G75" s="39"/>
+    <row r="72" spans="1:13" ht="30" thickTop="1" thickBot="1">
+      <c r="B72" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F72" s="24"/>
+      <c r="G72" s="24"/>
+      <c r="H72" s="23"/>
+      <c r="I72" s="26"/>
+    </row>
+    <row r="73" spans="1:13" ht="30" thickTop="1" thickBot="1">
+      <c r="B73" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F73" s="24"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="23"/>
+      <c r="I73" s="26"/>
+    </row>
+    <row r="74" spans="1:13" ht="16" thickTop="1" thickBot="1">
+      <c r="B74" s="36"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27"/>
+      <c r="E74" s="27"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="24"/>
+      <c r="H74" s="23"/>
+      <c r="I74" s="26"/>
+    </row>
+    <row r="75" spans="1:13" ht="16" thickTop="1" thickBot="1">
+      <c r="B75" s="36"/>
+      <c r="C75" s="27"/>
+      <c r="D75" s="27"/>
+      <c r="E75" s="27"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="24"/>
+      <c r="H75" s="23"/>
+      <c r="I75" s="26"/>
     </row>
     <row r="76" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B76" s="36"/>
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
-      <c r="E76" s="27"/>
+      <c r="B76" s="34"/>
       <c r="F76" s="24"/>
       <c r="G76" s="47"/>
       <c r="H76" s="23"/>
@@ -1850,7 +1899,7 @@
     </row>
     <row r="77" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="B77" s="36"/>
-      <c r="C77" s="27"/>
+      <c r="C77" s="30"/>
       <c r="D77" s="27"/>
       <c r="E77" s="27"/>
       <c r="F77" s="24"/>
@@ -1859,51 +1908,53 @@
       <c r="I77" s="26"/>
     </row>
     <row r="78" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B78" s="34"/>
-      <c r="F78" s="39"/>
-      <c r="G78" s="39"/>
+      <c r="A78" s="15"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="37"/>
+      <c r="G78" s="37"/>
+      <c r="H78" s="38"/>
+      <c r="I78" s="20"/>
+      <c r="J78" s="16"/>
+      <c r="K78" s="16"/>
+      <c r="L78" s="16"/>
+      <c r="M78" s="16"/>
     </row>
     <row r="79" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B79" s="36"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
-      <c r="E79" s="27"/>
+      <c r="B79" s="34"/>
       <c r="F79" s="24"/>
       <c r="G79" s="24"/>
       <c r="H79" s="23"/>
       <c r="I79" s="26"/>
     </row>
     <row r="80" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B80" s="36"/>
-      <c r="C80" s="30"/>
+      <c r="B80" s="34"/>
       <c r="F80" s="24"/>
       <c r="G80" s="24"/>
       <c r="H80" s="23"/>
       <c r="I80" s="26"/>
     </row>
-    <row r="81" spans="1:13" s="46" customFormat="1" ht="16" thickTop="1" thickBot="1">
-      <c r="A81" s="41"/>
-      <c r="B81" s="48"/>
-      <c r="C81" s="42"/>
+    <row r="81" spans="1:13" ht="16" thickTop="1" thickBot="1">
+      <c r="B81" s="36"/>
+      <c r="C81" s="27"/>
       <c r="D81" s="27"/>
       <c r="E81" s="27"/>
-      <c r="F81" s="43"/>
-      <c r="G81" s="43"/>
-      <c r="H81" s="44"/>
-      <c r="I81" s="45"/>
-    </row>
-    <row r="82" spans="1:13" s="46" customFormat="1" ht="16" thickTop="1" thickBot="1">
-      <c r="A82" s="41"/>
-      <c r="B82" s="48"/>
-      <c r="C82" s="42"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="27"/>
-      <c r="F82" s="43"/>
-      <c r="G82" s="43"/>
-      <c r="H82" s="44"/>
-      <c r="I82" s="45"/>
-    </row>
-    <row r="83" spans="1:13" s="46" customFormat="1" ht="60" customHeight="1" thickTop="1" thickBot="1">
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
+      <c r="H81" s="23"/>
+      <c r="I81" s="26"/>
+    </row>
+    <row r="82" spans="1:13" ht="16" thickTop="1" thickBot="1">
+      <c r="B82" s="36"/>
+      <c r="C82" s="30"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="24"/>
+      <c r="H82" s="23"/>
+      <c r="I82" s="26"/>
+    </row>
+    <row r="83" spans="1:13" s="46" customFormat="1" ht="16" thickTop="1" thickBot="1">
       <c r="A83" s="41"/>
       <c r="B83" s="48"/>
       <c r="C83" s="42"/>
@@ -1914,48 +1965,70 @@
       <c r="H83" s="44"/>
       <c r="I83" s="45"/>
     </row>
-    <row r="84" spans="1:13" ht="36" customHeight="1" thickTop="1">
-      <c r="A84" s="15"/>
-      <c r="B84" s="16"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="37"/>
-      <c r="G84" s="37"/>
-      <c r="H84" s="38"/>
-      <c r="I84" s="20"/>
-      <c r="J84" s="16"/>
-      <c r="K84" s="16"/>
-      <c r="L84" s="16"/>
-      <c r="M84" s="16"/>
-    </row>
-    <row r="85" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
-      <c r="B85" s="49"/>
-      <c r="C85" s="50"/>
-      <c r="F85" s="39"/>
-      <c r="G85" s="39"/>
-    </row>
-    <row r="86" spans="1:13" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B86" s="51"/>
-      <c r="F86" s="24"/>
-      <c r="G86" s="24"/>
-      <c r="H86" s="23"/>
-      <c r="I86" s="26"/>
-    </row>
-    <row r="87" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A87" s="15"/>
-      <c r="B87" s="16"/>
-      <c r="C87" s="17"/>
-      <c r="D87" s="17"/>
-      <c r="E87" s="18"/>
-      <c r="F87" s="52"/>
-      <c r="G87" s="52"/>
-      <c r="H87" s="53"/>
-      <c r="I87" s="54"/>
-      <c r="J87" s="16"/>
-      <c r="K87" s="16"/>
-      <c r="L87" s="16"/>
-      <c r="M87" s="16"/>
+    <row r="84" spans="1:13" s="46" customFormat="1" ht="16" thickTop="1" thickBot="1">
+      <c r="A84" s="41"/>
+      <c r="B84" s="48"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="27"/>
+      <c r="E84" s="27"/>
+      <c r="F84" s="43"/>
+      <c r="G84" s="43"/>
+      <c r="H84" s="44"/>
+      <c r="I84" s="45"/>
+    </row>
+    <row r="85" spans="1:13" s="46" customFormat="1" ht="60" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A85" s="41"/>
+      <c r="B85" s="48"/>
+      <c r="C85" s="42"/>
+      <c r="D85" s="27"/>
+      <c r="E85" s="27"/>
+      <c r="F85" s="43"/>
+      <c r="G85" s="43"/>
+      <c r="H85" s="44"/>
+      <c r="I85" s="45"/>
+    </row>
+    <row r="86" spans="1:13" ht="36" customHeight="1" thickTop="1">
+      <c r="A86" s="15"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="37"/>
+      <c r="G86" s="37"/>
+      <c r="H86" s="38"/>
+      <c r="I86" s="20"/>
+      <c r="J86" s="16"/>
+      <c r="K86" s="16"/>
+      <c r="L86" s="16"/>
+      <c r="M86" s="16"/>
+    </row>
+    <row r="87" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
+      <c r="B87" s="49"/>
+      <c r="C87" s="50"/>
+      <c r="F87" s="39"/>
+      <c r="G87" s="39"/>
+    </row>
+    <row r="88" spans="1:13" ht="45" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B88" s="51"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="24"/>
+      <c r="H88" s="23"/>
+      <c r="I88" s="26"/>
+    </row>
+    <row r="89" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A89" s="15"/>
+      <c r="B89" s="16"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="52"/>
+      <c r="G89" s="52"/>
+      <c r="H89" s="53"/>
+      <c r="I89" s="54"/>
+      <c r="J89" s="16"/>
+      <c r="K89" s="16"/>
+      <c r="L89" s="16"/>
+      <c r="M89" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
reporting to steering committee and a series of test results
git-svn-id: svn://localhost/ARK/trunk@8244 35ee9b83-dd2c-47f4-99a2-c706670c48ce
</commit_message>
<xml_diff>
--- a/usefulTools/TestFilesAndDocuments/UAT_Reporting_Data_Linkage_Requirements_no_results.xlsx
+++ b/usefulTools/TestFilesAndDocuments/UAT_Reporting_Data_Linkage_Requirements_no_results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
   <si>
     <t>Result coding: 1 = Pass (full functionality with no unexpected errors), 0 = Fail (lack of required functionality or reproducible error during testing), 9 = Conditional (partial functionality, error during testing which cannot be reproduced, poor user experience or other constraints) X = Functionality which is desirable for future iterations of the system. these items are not necessary for user acceptance of this version of the system</t>
   </si>
@@ -140,9 +140,6 @@
     <t>1.12</t>
   </si>
   <si>
-    <t>alter consent to specific components and see that it appopriately increments and decrements the component-specific-constent counts</t>
-  </si>
-  <si>
     <t>Study-level Consent Details Report</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
     <t>Biospecimen Summary Report Report</t>
   </si>
   <si>
-    <t>a user with appropriate access rights can access the Biospecimen Summar Report</t>
-  </si>
-  <si>
     <t>a user withOUT appropriate access rights can NOT access the Biospecimen Summary Report</t>
   </si>
   <si>
@@ -222,16 +216,68 @@
   </si>
   <si>
     <t xml:space="preserve">  This report lists the biospecimen study details for the selected study - including location information.  It is essentially the same as the biospecimen summary report but includes the detailled location/inventory information related to each biospecimen (it is worth noting it will take a little longer too as a result)</t>
+  </si>
+  <si>
+    <t>ARK-xx It seems that the sub-headings are not showing up in our production environment for the Study Summary Report</t>
+  </si>
+  <si>
+    <t>AR-xxx - hide reporting from users without reporting permissions</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>If they can read only the study they can read the summary</t>
+  </si>
+  <si>
+    <t>Can't yet remove access once given so can't test</t>
+  </si>
+  <si>
+    <t>Counts archived ie deleted cases</t>
+  </si>
+  <si>
+    <t>deleted subjects with allocated biospecs, number doesn't change but it becomes archived which you see is study summary report</t>
+  </si>
+  <si>
+    <t>alter consent to specific components and see that it appopriately increments and decrements the component-specific-consent counts</t>
+  </si>
+  <si>
+    <t>ARK-1050 currently included archived subjects but will change and label accordingly</t>
+  </si>
+  <si>
+    <t>Used sleep study to check components</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>no labels on report</t>
+  </si>
+  <si>
+    <t>a user with appropriate access rights can access the Biospecimen Detail Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">but it included archived subject who had biospecs when archived </t>
+  </si>
+  <si>
+    <t>a user with appropriate access rights can access the Biospecimen Summary Report</t>
+  </si>
+  <si>
+    <t>going to add sample date and collectin ID, in JIRA</t>
+  </si>
+  <si>
+    <t>report includes biospecs from archived subjects</t>
+  </si>
+  <si>
+    <t>10/7/2013  13::00 AM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="d/mm/yyyy\ h:mm"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy\ hh:mm"/>
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -396,7 +442,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -416,8 +462,26 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -491,18 +555,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -557,9 +615,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -584,8 +639,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -595,6 +677,15 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -604,6 +695,15 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1003,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMF89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1012,19 +1112,20 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="74.33203125" style="2" customWidth="1"/>
     <col min="3" max="5" width="7.5" style="3" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="4"/>
+    <col min="6" max="6" width="10.83203125" style="4"/>
+    <col min="7" max="7" width="14.83203125" style="53" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="5"/>
     <col min="9" max="9" width="10.83203125" style="6"/>
     <col min="13" max="1020" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="69" customHeight="1">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" customHeight="1">
       <c r="B2" s="9"/>
@@ -1051,7 +1152,7 @@
       <c r="F3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="54" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -1068,7 +1169,7 @@
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
       <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="19"/>
       <c r="I4" s="20"/>
       <c r="J4" s="16"/>
@@ -1084,10 +1185,10 @@
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
       <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
+      <c r="G5" s="56"/>
       <c r="H5" s="23"/>
     </row>
-    <row r="6" spans="1:13" ht="86">
+    <row r="6" spans="1:13" ht="84">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1097,12 +1198,18 @@
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="26"/>
-    </row>
-    <row r="7" spans="1:13" ht="16">
+      <c r="F6" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="57">
+        <v>41554.5</v>
+      </c>
+      <c r="H6" s="23">
+        <v>1</v>
+      </c>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1110,14 +1217,20 @@
         <v>14</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="26"/>
-    </row>
-    <row r="8" spans="1:13" ht="16">
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="57">
+        <v>41554.510416666664</v>
+      </c>
+      <c r="H7" s="23">
+        <v>1</v>
+      </c>
+      <c r="I7" s="25"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1125,14 +1238,23 @@
         <v>16</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="26"/>
-    </row>
-    <row r="9" spans="1:13" ht="16">
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="57">
+        <v>41554.510416666664</v>
+      </c>
+      <c r="H8" s="23">
+        <v>1</v>
+      </c>
+      <c r="I8" s="25"/>
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1140,14 +1262,23 @@
         <v>18</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="26"/>
-    </row>
-    <row r="10" spans="1:13" ht="16">
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="57">
+        <v>41554.510416666664</v>
+      </c>
+      <c r="H9" s="23">
+        <v>1</v>
+      </c>
+      <c r="I9" s="25"/>
+      <c r="J9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1155,14 +1286,23 @@
         <v>20</v>
       </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="26"/>
-    </row>
-    <row r="11" spans="1:13" ht="16">
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="27">
+        <v>9</v>
+      </c>
+      <c r="I10" s="25"/>
+      <c r="J10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1172,396 +1312,519 @@
       <c r="C11" s="9"/>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="26"/>
-    </row>
-    <row r="12" spans="1:13" ht="16">
+      <c r="F11" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="27">
+        <v>9</v>
+      </c>
+      <c r="I11" s="25"/>
+      <c r="J11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="26"/>
-    </row>
-    <row r="13" spans="1:13" ht="16">
+      <c r="C12" s="28"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="57">
+        <v>41554.513888888891</v>
+      </c>
+      <c r="H12" s="27">
+        <v>1</v>
+      </c>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="26"/>
-    </row>
-    <row r="14" spans="1:13" ht="30">
+      <c r="C13" s="28"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="57">
+        <v>41554.517361111109</v>
+      </c>
+      <c r="H13" s="29">
+        <v>1</v>
+      </c>
+      <c r="I13" s="25"/>
+      <c r="J13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="28">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="26"/>
-    </row>
-    <row r="15" spans="1:13" ht="30">
+      <c r="C14" s="28"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="57">
+        <v>41554.52847222222</v>
+      </c>
+      <c r="H14" s="27">
+        <v>1</v>
+      </c>
+      <c r="I14" s="25"/>
+    </row>
+    <row r="15" spans="1:13" ht="28">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="26"/>
-    </row>
-    <row r="16" spans="1:13" ht="30">
+      <c r="C15" s="28"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="57">
+        <v>41554.53125</v>
+      </c>
+      <c r="H15" s="27">
+        <v>1</v>
+      </c>
+      <c r="I15" s="25"/>
+      <c r="J15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="28">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="26"/>
-    </row>
-    <row r="17" spans="1:9" ht="30">
+      <c r="C16" s="28"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="57">
+        <v>41554.539583333331</v>
+      </c>
+      <c r="H16" s="27">
+        <v>1</v>
+      </c>
+      <c r="I16" s="25"/>
+      <c r="J16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="28">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="26"/>
-    </row>
-    <row r="18" spans="1:9" ht="16">
-      <c r="B18" s="30"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
+      <c r="F17" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="27">
+        <v>1</v>
+      </c>
+      <c r="I17" s="25"/>
+      <c r="J17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="28"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
       <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="26"/>
-    </row>
-    <row r="19" spans="1:9" ht="16">
-      <c r="B19" s="32" t="s">
+      <c r="G18" s="57"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="25"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="B19" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="25"/>
+    </row>
+    <row r="20" spans="1:10" ht="30" thickTop="1" thickBot="1">
+      <c r="B20" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="26"/>
-    </row>
-    <row r="20" spans="1:9" ht="30" thickTop="1" thickBot="1">
-      <c r="B20" s="21" t="s">
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="57">
+        <v>41554.545138888891</v>
+      </c>
+      <c r="H20" s="27">
+        <v>1</v>
+      </c>
+      <c r="I20" s="25"/>
+    </row>
+    <row r="21" spans="1:10" ht="16" thickTop="1" thickBot="1">
+      <c r="B21" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="26"/>
-    </row>
-    <row r="21" spans="1:9" ht="16" thickTop="1" thickBot="1">
-      <c r="B21" s="9" t="s">
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="57">
+        <v>41554.554861111108</v>
+      </c>
+      <c r="H21" s="27">
+        <v>1</v>
+      </c>
+      <c r="I21" s="25"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="B22" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="26"/>
-    </row>
-    <row r="22" spans="1:9" ht="16">
-      <c r="B22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="26"/>
-    </row>
-    <row r="23" spans="1:9" ht="16">
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="31"/>
+      <c r="I22" s="25"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="B23" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="26"/>
-    </row>
-    <row r="24" spans="1:9" ht="30">
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="27"/>
+      <c r="I23" s="25"/>
+    </row>
+    <row r="24" spans="1:10" ht="28">
       <c r="B24" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="57">
+        <v>41554.556250000001</v>
+      </c>
+      <c r="H24" s="27">
+        <v>1</v>
+      </c>
+      <c r="I24" s="25"/>
+    </row>
+    <row r="25" spans="1:10" ht="28">
+      <c r="B25" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="26"/>
-    </row>
-    <row r="25" spans="1:9" ht="30">
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="57">
+        <v>41554.557638888888</v>
+      </c>
+      <c r="H25" s="27">
+        <v>1</v>
+      </c>
+      <c r="I25" s="25"/>
+    </row>
+    <row r="26" spans="1:10" ht="28">
+      <c r="B26" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="26"/>
-    </row>
-    <row r="26" spans="1:9" ht="30">
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="57">
+        <v>41554.558333333334</v>
+      </c>
+      <c r="H26" s="31">
+        <v>1</v>
+      </c>
+      <c r="I26" s="25"/>
+    </row>
+    <row r="27" spans="1:10" ht="56">
+      <c r="B27" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="26"/>
-    </row>
-    <row r="27" spans="1:9" ht="58">
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="57">
+        <v>41554.560416666667</v>
+      </c>
+      <c r="H27" s="31">
+        <v>1</v>
+      </c>
+      <c r="I27" s="25"/>
+    </row>
+    <row r="28" spans="1:10" ht="28">
+      <c r="B28" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="26"/>
-    </row>
-    <row r="28" spans="1:9" ht="30">
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="57">
+        <v>41554.561111111114</v>
+      </c>
+      <c r="H28" s="27">
+        <v>1</v>
+      </c>
+      <c r="I28" s="25"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="25"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="B30" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="26"/>
-    </row>
-    <row r="29" spans="1:9" ht="16">
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="26"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="B30" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
       <c r="F30" s="24"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="26"/>
-    </row>
-    <row r="31" spans="1:9" ht="30" thickTop="1" thickBot="1">
+      <c r="G30" s="57"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="25"/>
+    </row>
+    <row r="31" spans="1:10" ht="30" thickTop="1" thickBot="1">
       <c r="B31" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="25"/>
+    </row>
+    <row r="32" spans="1:10" ht="16" thickTop="1" thickBot="1">
+      <c r="B32" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="26"/>
-    </row>
-    <row r="32" spans="1:9" ht="16" thickTop="1" thickBot="1">
-      <c r="B32" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G32" s="57"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="25"/>
     </row>
     <row r="33" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="B33" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="26"/>
+        <v>37</v>
+      </c>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G33" s="57"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="25"/>
     </row>
     <row r="34" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="B34" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" s="57"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="25"/>
     </row>
     <row r="35" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B35" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="26"/>
+        <v>38</v>
+      </c>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G35" s="57"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B36" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
+        <v>39</v>
+      </c>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G36" s="56"/>
     </row>
     <row r="37" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B37" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="26"/>
+        <v>40</v>
+      </c>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G37" s="57"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="25"/>
     </row>
     <row r="38" spans="1:13" ht="58" thickTop="1" thickBot="1">
       <c r="B38" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="26"/>
+        <v>41</v>
+      </c>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G38" s="57"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="25"/>
     </row>
     <row r="39" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B39" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="26"/>
+        <v>42</v>
+      </c>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G39" s="57"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="25"/>
     </row>
     <row r="40" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B40" s="36"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
       <c r="F40" s="24"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="26"/>
+      <c r="G40" s="57"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="25"/>
     </row>
     <row r="41" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B41" s="36"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
       <c r="F41" s="24"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="26"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="25"/>
     </row>
     <row r="42" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B42" s="36"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
       <c r="F42" s="24"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="26"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="25"/>
     </row>
     <row r="43" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B43" s="36"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
       <c r="F43" s="24"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="26"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="25"/>
     </row>
     <row r="44" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="A44" s="15"/>
@@ -1569,9 +1832,9 @@
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
       <c r="E44" s="18"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="38"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="36"/>
       <c r="I44" s="20"/>
       <c r="J44" s="16"/>
       <c r="K44" s="16"/>
@@ -1580,63 +1843,73 @@
     </row>
     <row r="45" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="A45" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
+      <c r="G45" s="57"/>
       <c r="H45" s="23"/>
-      <c r="I45" s="26"/>
+      <c r="I45" s="25"/>
     </row>
     <row r="46" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B46" s="32" t="s">
-        <v>46</v>
+      <c r="B46" s="30" t="s">
+        <v>45</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="26"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="25"/>
     </row>
     <row r="47" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="B47" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
+      <c r="G47" s="57"/>
       <c r="H47" s="23"/>
-      <c r="I47" s="26"/>
+      <c r="I47" s="25"/>
     </row>
     <row r="48" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="B48" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="26"/>
+      <c r="F48" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G48" s="57">
+        <v>41554.563194444447</v>
+      </c>
+      <c r="H48" s="23">
+        <v>1</v>
+      </c>
+      <c r="I48" s="25"/>
     </row>
     <row r="49" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B49" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="26"/>
+      <c r="F49" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G49" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="H49" s="38"/>
+      <c r="I49" s="25"/>
     </row>
     <row r="50" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="B50" s="9" t="s">
@@ -1645,54 +1918,72 @@
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
+      <c r="F50" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G50" s="57" t="s">
+        <v>70</v>
+      </c>
       <c r="H50" s="23"/>
-      <c r="I50" s="26"/>
+      <c r="I50" s="25"/>
     </row>
     <row r="51" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B51" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="23"/>
-      <c r="I51" s="26"/>
+      <c r="F51" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G51" s="57">
+        <v>41554.564583333333</v>
+      </c>
+      <c r="H51" s="23">
+        <v>1</v>
+      </c>
+      <c r="I51" s="25"/>
     </row>
     <row r="52" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B52" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="26"/>
+      <c r="F52" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G52" s="57">
+        <v>41554.567361111112</v>
+      </c>
+      <c r="H52" s="38">
+        <v>1</v>
+      </c>
+      <c r="I52" s="25" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="53" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B53" s="51"/>
+      <c r="B53" s="48"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
+      <c r="G53" s="57"/>
       <c r="H53" s="23"/>
-      <c r="I53" s="26"/>
+      <c r="I53" s="25"/>
     </row>
     <row r="54" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B54" s="34"/>
+      <c r="B54" s="32"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
+      <c r="G54" s="57"/>
       <c r="H54" s="23"/>
-      <c r="I54" s="26"/>
+      <c r="I54" s="25"/>
     </row>
     <row r="55" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="A55" s="15"/>
@@ -1700,9 +1991,9 @@
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
       <c r="E55" s="18"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="37"/>
-      <c r="H55" s="38"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="36"/>
       <c r="I55" s="20"/>
       <c r="J55" s="16"/>
       <c r="K55" s="16"/>
@@ -1711,201 +2002,275 @@
     </row>
     <row r="56" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="A56" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56" s="32"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="57"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="25"/>
+    </row>
+    <row r="57" spans="1:13" ht="16" thickTop="1" thickBot="1">
+      <c r="B57" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B56" s="34"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="23"/>
-      <c r="I56" s="26"/>
-    </row>
-    <row r="57" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B57" s="32" t="s">
-        <v>53</v>
-      </c>
       <c r="F57" s="24"/>
-      <c r="G57" s="47"/>
+      <c r="G57" s="57"/>
       <c r="H57" s="23"/>
-      <c r="I57" s="26"/>
+      <c r="I57" s="25"/>
     </row>
     <row r="58" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B58" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F58" s="24"/>
-      <c r="G58" s="47"/>
+      <c r="G58" s="57"/>
       <c r="H58" s="23"/>
-      <c r="I58" s="26"/>
+      <c r="I58" s="25"/>
     </row>
     <row r="59" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="B59" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F59" s="24"/>
-      <c r="G59" s="47"/>
-      <c r="H59" s="23"/>
-      <c r="I59" s="26"/>
+        <v>74</v>
+      </c>
+      <c r="F59" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G59" s="57">
+        <v>41554.572222222225</v>
+      </c>
+      <c r="H59" s="23">
+        <v>1</v>
+      </c>
+      <c r="I59" s="25"/>
     </row>
     <row r="60" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="B60" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F60" s="24"/>
-      <c r="G60" s="47"/>
+        <v>53</v>
+      </c>
+      <c r="F60" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G60" s="57" t="s">
+        <v>70</v>
+      </c>
       <c r="H60" s="23"/>
-      <c r="I60" s="26"/>
+      <c r="I60" s="25"/>
     </row>
     <row r="61" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B61" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F61" s="24"/>
-      <c r="G61" s="47"/>
-      <c r="H61" s="23"/>
-      <c r="I61" s="26"/>
+        <v>54</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G61" s="57">
+        <v>41554.573611111111</v>
+      </c>
+      <c r="H61" s="23">
+        <v>1</v>
+      </c>
+      <c r="I61" s="25"/>
     </row>
     <row r="62" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B62" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F62" s="24"/>
-      <c r="G62" s="47"/>
-      <c r="H62" s="23"/>
-      <c r="I62" s="26"/>
-    </row>
-    <row r="63" spans="1:13" ht="30" thickTop="1" thickBot="1">
+        <v>56</v>
+      </c>
+      <c r="F62" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G62" s="57">
+        <v>41554.579861111109</v>
+      </c>
+      <c r="H62" s="23">
+        <v>1</v>
+      </c>
+      <c r="I62" s="25"/>
+    </row>
+    <row r="63" spans="1:13" ht="114" thickTop="1" thickBot="1">
       <c r="B63" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F63" s="24"/>
-      <c r="G63" s="47"/>
-      <c r="H63" s="23"/>
-      <c r="I63" s="26"/>
+        <v>55</v>
+      </c>
+      <c r="F63" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G63" s="57">
+        <v>41554.584722222222</v>
+      </c>
+      <c r="H63" s="23">
+        <v>1</v>
+      </c>
+      <c r="I63" s="25" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="64" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B64" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F64" s="24"/>
-      <c r="G64" s="47"/>
-      <c r="H64" s="23"/>
-      <c r="I64" s="26"/>
+        <v>57</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G64" s="57">
+        <v>41554.586111111108</v>
+      </c>
+      <c r="H64" s="23">
+        <v>1</v>
+      </c>
+      <c r="I64" s="25"/>
     </row>
     <row r="65" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="B65" s="8"/>
       <c r="F65" s="24"/>
-      <c r="G65" s="47"/>
+      <c r="G65" s="57"/>
       <c r="H65" s="23"/>
-      <c r="I65" s="26"/>
+      <c r="I65" s="25"/>
     </row>
     <row r="66" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B66" s="32" t="s">
-        <v>60</v>
+      <c r="B66" s="30" t="s">
+        <v>58</v>
       </c>
       <c r="F66" s="24"/>
-      <c r="G66" s="24"/>
+      <c r="G66" s="57"/>
       <c r="H66" s="23"/>
-      <c r="I66" s="26"/>
-    </row>
-    <row r="67" spans="1:13" ht="58" thickTop="1" thickBot="1">
+      <c r="I66" s="25"/>
+    </row>
+    <row r="67" spans="1:13" ht="72" thickTop="1" thickBot="1">
       <c r="B67" s="21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F67" s="24"/>
-      <c r="G67" s="24"/>
+      <c r="G67" s="57"/>
       <c r="H67" s="23"/>
-      <c r="I67" s="26"/>
-    </row>
-    <row r="68" spans="1:13" ht="16" thickTop="1" thickBot="1">
+      <c r="I67" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="86" thickTop="1" thickBot="1">
       <c r="B68" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F68" s="24"/>
-      <c r="G68" s="24"/>
-      <c r="H68" s="23"/>
-      <c r="I68" s="26"/>
+        <v>72</v>
+      </c>
+      <c r="F68" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G68" s="57">
+        <v>41554.587500000001</v>
+      </c>
+      <c r="H68" s="23">
+        <v>1</v>
+      </c>
+      <c r="I68" s="25" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="69" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="B69" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F69" s="24"/>
-      <c r="G69" s="24"/>
+        <v>53</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G69" s="57" t="s">
+        <v>70</v>
+      </c>
       <c r="H69" s="23"/>
-      <c r="I69" s="26"/>
+      <c r="I69" s="25"/>
     </row>
     <row r="70" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B70" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F70" s="24"/>
-      <c r="G70" s="24"/>
-      <c r="H70" s="23"/>
-      <c r="I70" s="26"/>
+        <v>54</v>
+      </c>
+      <c r="F70" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G70" s="57">
+        <v>41554.589583333334</v>
+      </c>
+      <c r="H70" s="23">
+        <v>1</v>
+      </c>
+      <c r="I70" s="25"/>
     </row>
     <row r="71" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B71" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="23"/>
-      <c r="I71" s="26"/>
+        <v>56</v>
+      </c>
+      <c r="F71" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G71" s="57">
+        <v>41554.59097222222</v>
+      </c>
+      <c r="H71" s="23">
+        <v>1</v>
+      </c>
+      <c r="I71" s="25"/>
     </row>
     <row r="72" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B72" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F72" s="24"/>
-      <c r="G72" s="24"/>
-      <c r="H72" s="23"/>
-      <c r="I72" s="26"/>
+        <v>55</v>
+      </c>
+      <c r="F72" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G72" s="57">
+        <v>41554.593055555553</v>
+      </c>
+      <c r="H72" s="23">
+        <v>1</v>
+      </c>
+      <c r="I72" s="25"/>
     </row>
     <row r="73" spans="1:13" ht="30" thickTop="1" thickBot="1">
       <c r="B73" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F73" s="24"/>
-      <c r="G73" s="24"/>
-      <c r="H73" s="23"/>
-      <c r="I73" s="26"/>
+        <v>57</v>
+      </c>
+      <c r="F73" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G73" s="57">
+        <v>41554.59375</v>
+      </c>
+      <c r="H73" s="23">
+        <v>1</v>
+      </c>
+      <c r="I73" s="25"/>
     </row>
     <row r="74" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B74" s="36"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
-      <c r="E74" s="27"/>
+      <c r="B74" s="34"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
       <c r="F74" s="24"/>
-      <c r="G74" s="24"/>
+      <c r="G74" s="57"/>
       <c r="H74" s="23"/>
-      <c r="I74" s="26"/>
+      <c r="I74" s="25"/>
     </row>
     <row r="75" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B75" s="36"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="27"/>
+      <c r="B75" s="34"/>
+      <c r="C75" s="26"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="26"/>
       <c r="F75" s="24"/>
-      <c r="G75" s="24"/>
+      <c r="G75" s="57"/>
       <c r="H75" s="23"/>
-      <c r="I75" s="26"/>
+      <c r="I75" s="25"/>
     </row>
     <row r="76" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B76" s="34"/>
+      <c r="B76" s="32"/>
       <c r="F76" s="24"/>
-      <c r="G76" s="47"/>
+      <c r="G76" s="57"/>
       <c r="H76" s="23"/>
-      <c r="I76" s="26"/>
+      <c r="I76" s="25"/>
     </row>
     <row r="77" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B77" s="36"/>
-      <c r="C77" s="30"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="27"/>
+      <c r="B77" s="34"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="26"/>
+      <c r="E77" s="26"/>
       <c r="F77" s="24"/>
-      <c r="G77" s="47"/>
+      <c r="G77" s="57"/>
       <c r="H77" s="23"/>
-      <c r="I77" s="26"/>
+      <c r="I77" s="25"/>
     </row>
     <row r="78" spans="1:13" ht="16" thickTop="1" thickBot="1">
       <c r="A78" s="15"/>
@@ -1913,9 +2278,9 @@
       <c r="C78" s="17"/>
       <c r="D78" s="17"/>
       <c r="E78" s="18"/>
-      <c r="F78" s="37"/>
-      <c r="G78" s="37"/>
-      <c r="H78" s="38"/>
+      <c r="F78" s="35"/>
+      <c r="G78" s="58"/>
+      <c r="H78" s="36"/>
       <c r="I78" s="20"/>
       <c r="J78" s="16"/>
       <c r="K78" s="16"/>
@@ -1923,69 +2288,69 @@
       <c r="M78" s="16"/>
     </row>
     <row r="79" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B79" s="34"/>
+      <c r="B79" s="32"/>
       <c r="F79" s="24"/>
-      <c r="G79" s="24"/>
+      <c r="G79" s="57"/>
       <c r="H79" s="23"/>
-      <c r="I79" s="26"/>
+      <c r="I79" s="25"/>
     </row>
     <row r="80" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B80" s="34"/>
+      <c r="B80" s="32"/>
       <c r="F80" s="24"/>
-      <c r="G80" s="24"/>
+      <c r="G80" s="57"/>
       <c r="H80" s="23"/>
-      <c r="I80" s="26"/>
+      <c r="I80" s="25"/>
     </row>
     <row r="81" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B81" s="36"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27"/>
+      <c r="B81" s="34"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
+      <c r="E81" s="26"/>
       <c r="F81" s="24"/>
-      <c r="G81" s="24"/>
+      <c r="G81" s="57"/>
       <c r="H81" s="23"/>
-      <c r="I81" s="26"/>
+      <c r="I81" s="25"/>
     </row>
     <row r="82" spans="1:13" ht="16" thickTop="1" thickBot="1">
-      <c r="B82" s="36"/>
-      <c r="C82" s="30"/>
+      <c r="B82" s="34"/>
+      <c r="C82" s="28"/>
       <c r="F82" s="24"/>
-      <c r="G82" s="24"/>
+      <c r="G82" s="57"/>
       <c r="H82" s="23"/>
-      <c r="I82" s="26"/>
-    </row>
-    <row r="83" spans="1:13" s="46" customFormat="1" ht="16" thickTop="1" thickBot="1">
-      <c r="A83" s="41"/>
-      <c r="B83" s="48"/>
-      <c r="C83" s="42"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="43"/>
-      <c r="G83" s="43"/>
-      <c r="H83" s="44"/>
-      <c r="I83" s="45"/>
-    </row>
-    <row r="84" spans="1:13" s="46" customFormat="1" ht="16" thickTop="1" thickBot="1">
-      <c r="A84" s="41"/>
-      <c r="B84" s="48"/>
-      <c r="C84" s="42"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="43"/>
-      <c r="H84" s="44"/>
-      <c r="I84" s="45"/>
-    </row>
-    <row r="85" spans="1:13" s="46" customFormat="1" ht="60" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A85" s="41"/>
-      <c r="B85" s="48"/>
-      <c r="C85" s="42"/>
-      <c r="D85" s="27"/>
-      <c r="E85" s="27"/>
-      <c r="F85" s="43"/>
-      <c r="G85" s="43"/>
-      <c r="H85" s="44"/>
-      <c r="I85" s="45"/>
+      <c r="I82" s="25"/>
+    </row>
+    <row r="83" spans="1:13" s="44" customFormat="1" ht="16" thickTop="1" thickBot="1">
+      <c r="A83" s="39"/>
+      <c r="B83" s="45"/>
+      <c r="C83" s="40"/>
+      <c r="D83" s="26"/>
+      <c r="E83" s="26"/>
+      <c r="F83" s="41"/>
+      <c r="G83" s="59"/>
+      <c r="H83" s="42"/>
+      <c r="I83" s="43"/>
+    </row>
+    <row r="84" spans="1:13" s="44" customFormat="1" ht="16" thickTop="1" thickBot="1">
+      <c r="A84" s="39"/>
+      <c r="B84" s="45"/>
+      <c r="C84" s="40"/>
+      <c r="D84" s="26"/>
+      <c r="E84" s="26"/>
+      <c r="F84" s="41"/>
+      <c r="G84" s="59"/>
+      <c r="H84" s="42"/>
+      <c r="I84" s="43"/>
+    </row>
+    <row r="85" spans="1:13" s="44" customFormat="1" ht="60" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A85" s="39"/>
+      <c r="B85" s="45"/>
+      <c r="C85" s="40"/>
+      <c r="D85" s="26"/>
+      <c r="E85" s="26"/>
+      <c r="F85" s="41"/>
+      <c r="G85" s="59"/>
+      <c r="H85" s="42"/>
+      <c r="I85" s="43"/>
     </row>
     <row r="86" spans="1:13" ht="36" customHeight="1" thickTop="1">
       <c r="A86" s="15"/>
@@ -1993,9 +2358,9 @@
       <c r="C86" s="17"/>
       <c r="D86" s="17"/>
       <c r="E86" s="18"/>
-      <c r="F86" s="37"/>
-      <c r="G86" s="37"/>
-      <c r="H86" s="38"/>
+      <c r="F86" s="35"/>
+      <c r="G86" s="58"/>
+      <c r="H86" s="36"/>
       <c r="I86" s="20"/>
       <c r="J86" s="16"/>
       <c r="K86" s="16"/>
@@ -2003,17 +2368,17 @@
       <c r="M86" s="16"/>
     </row>
     <row r="87" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
-      <c r="B87" s="49"/>
-      <c r="C87" s="50"/>
-      <c r="F87" s="39"/>
-      <c r="G87" s="39"/>
+      <c r="B87" s="46"/>
+      <c r="C87" s="47"/>
+      <c r="F87" s="37"/>
+      <c r="G87" s="60"/>
     </row>
     <row r="88" spans="1:13" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B88" s="51"/>
+      <c r="B88" s="48"/>
       <c r="F88" s="24"/>
-      <c r="G88" s="24"/>
+      <c r="G88" s="57"/>
       <c r="H88" s="23"/>
-      <c r="I88" s="26"/>
+      <c r="I88" s="25"/>
     </row>
     <row r="89" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1">
       <c r="A89" s="15"/>
@@ -2021,10 +2386,10 @@
       <c r="C89" s="17"/>
       <c r="D89" s="17"/>
       <c r="E89" s="18"/>
-      <c r="F89" s="52"/>
-      <c r="G89" s="52"/>
-      <c r="H89" s="53"/>
-      <c r="I89" s="54"/>
+      <c r="F89" s="49"/>
+      <c r="G89" s="61"/>
+      <c r="H89" s="50"/>
+      <c r="I89" s="51"/>
       <c r="J89" s="16"/>
       <c r="K89" s="16"/>
       <c r="L89" s="16"/>

</xml_diff>